<commit_message>
Update Project Sheet Listing + move files
</commit_message>
<xml_diff>
--- a/# DOSSIER FINAL #/Administration_Projet/A1_Fondamentaux_Scientifiques_2017_2018_PROJET_Grille_Evaluation_ETUDIANT.xlsx
+++ b/# DOSSIER FINAL #/Administration_Projet/A1_Fondamentaux_Scientifiques_2017_2018_PROJET_Grille_Evaluation_ETUDIANT.xlsx
@@ -1681,8 +1681,8 @@
   </sheetPr>
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1985,7 +1985,7 @@
       <c r="C29" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="12" t="s">
         <v>56</v>
       </c>
       <c r="E29" s="44"/>
@@ -2012,7 +2012,7 @@
       <c r="A32" s="53"/>
       <c r="B32" s="53"/>
       <c r="C32" s="53"/>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="12" t="s">
         <v>61</v>
       </c>
       <c r="E32" s="9"/>
@@ -2021,7 +2021,7 @@
       <c r="A33" s="53"/>
       <c r="B33" s="53"/>
       <c r="C33" s="53"/>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="13" t="s">
         <v>66</v>
       </c>
       <c r="E33" s="9"/>
@@ -2039,7 +2039,7 @@
       <c r="A35" s="53"/>
       <c r="B35" s="53"/>
       <c r="C35" s="53"/>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="13" t="s">
         <v>59</v>
       </c>
       <c r="E35" s="9"/>
@@ -2061,7 +2061,7 @@
       <c r="C37" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="12" t="s">
         <v>79</v>
       </c>
       <c r="E37" s="10"/>
@@ -2121,7 +2121,7 @@
       <c r="A43" s="35"/>
       <c r="B43" s="36"/>
       <c r="C43" s="37"/>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="14" t="s">
         <v>60</v>
       </c>
       <c r="E43" s="44"/>

</xml_diff>